<commit_message>
add cased about complex data type
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2874" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2881" uniqueCount="1043">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3790,14 +3790,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>drop table negative_331_00_schema1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>truncate table negative_332_00_schema1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Error:  (state=90001,code=90001)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3854,6 +3846,29 @@
   </si>
   <si>
     <t>negative_316</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_333</t>
+  </si>
+  <si>
+    <t>drop table negative_332_00_schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>truncate table negative_333_00_schema1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建表，指定不允许为null的字段的默认值为null，应创建失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table negative_331(id int,name varchar(32) not null default null,age int,primary key(id))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error: Invalid default value for 'name'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4212,10 +4227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K333"/>
+  <dimension ref="A1:K334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
-      <selection activeCell="E301" sqref="E301"/>
+    <sheetView tabSelected="1" topLeftCell="A309" workbookViewId="0">
+      <selection activeCell="J332" sqref="J332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4257,7 +4272,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -4271,7 +4286,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>20</v>
@@ -4324,7 +4339,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>27</v>
@@ -4385,7 +4400,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>37</v>
@@ -4420,7 +4435,7 @@
         <v>15</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>40</v>
@@ -6683,7 +6698,7 @@
         <v>15</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>289</v>
@@ -10045,7 +10060,7 @@
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>25</v>
@@ -10086,7 +10101,7 @@
         <v>14</v>
       </c>
       <c r="H226" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I226" s="1" t="s">
         <v>670</v>
@@ -10115,7 +10130,7 @@
         <v>14</v>
       </c>
       <c r="H227" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I227" s="1" t="s">
         <v>671</v>
@@ -10144,7 +10159,7 @@
         <v>14</v>
       </c>
       <c r="H228" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I228" s="1" t="s">
         <v>672</v>
@@ -10173,7 +10188,7 @@
         <v>14</v>
       </c>
       <c r="H229" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I229" s="1" t="s">
         <v>673</v>
@@ -10202,7 +10217,7 @@
         <v>14</v>
       </c>
       <c r="H230" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I230" s="1" t="s">
         <v>674</v>
@@ -10231,7 +10246,7 @@
         <v>14</v>
       </c>
       <c r="H231" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I231" s="1" t="s">
         <v>676</v>
@@ -10260,7 +10275,7 @@
         <v>14</v>
       </c>
       <c r="H232" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I232" s="1" t="s">
         <v>675</v>
@@ -10289,7 +10304,7 @@
         <v>14</v>
       </c>
       <c r="H233" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I233" s="1" t="s">
         <v>677</v>
@@ -10318,7 +10333,7 @@
         <v>14</v>
       </c>
       <c r="H234" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I234" s="1" t="s">
         <v>679</v>
@@ -10347,7 +10362,7 @@
         <v>14</v>
       </c>
       <c r="H235" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>678</v>
@@ -10376,7 +10391,7 @@
         <v>14</v>
       </c>
       <c r="H236" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I236" s="1" t="s">
         <v>680</v>
@@ -10405,7 +10420,7 @@
         <v>14</v>
       </c>
       <c r="H237" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I237" s="1" t="s">
         <v>681</v>
@@ -10463,7 +10478,7 @@
         <v>15</v>
       </c>
       <c r="H239" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I239" s="1" t="s">
         <v>724</v>
@@ -10498,7 +10513,7 @@
         <v>15</v>
       </c>
       <c r="H240" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I240" s="1" t="s">
         <v>725</v>
@@ -10533,7 +10548,7 @@
         <v>15</v>
       </c>
       <c r="H241" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I241" s="1" t="s">
         <v>726</v>
@@ -10568,7 +10583,7 @@
         <v>15</v>
       </c>
       <c r="H242" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I242" s="1" t="s">
         <v>727</v>
@@ -10603,7 +10618,7 @@
         <v>15</v>
       </c>
       <c r="H243" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I243" s="1" t="s">
         <v>728</v>
@@ -10638,7 +10653,7 @@
         <v>15</v>
       </c>
       <c r="H244" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I244" s="1" t="s">
         <v>729</v>
@@ -10673,7 +10688,7 @@
         <v>15</v>
       </c>
       <c r="H245" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I245" s="1" t="s">
         <v>730</v>
@@ -10708,7 +10723,7 @@
         <v>15</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I246" s="1" t="s">
         <v>731</v>
@@ -10743,7 +10758,7 @@
         <v>15</v>
       </c>
       <c r="H247" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I247" s="1" t="s">
         <v>737</v>
@@ -10778,7 +10793,7 @@
         <v>15</v>
       </c>
       <c r="H248" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I248" s="1" t="s">
         <v>738</v>
@@ -10813,7 +10828,7 @@
         <v>15</v>
       </c>
       <c r="H249" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I249" s="1" t="s">
         <v>739</v>
@@ -10848,7 +10863,7 @@
         <v>15</v>
       </c>
       <c r="H250" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I250" s="1" t="s">
         <v>740</v>
@@ -10883,7 +10898,7 @@
         <v>15</v>
       </c>
       <c r="H251" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I251" s="1" t="s">
         <v>741</v>
@@ -10918,7 +10933,7 @@
         <v>15</v>
       </c>
       <c r="H252" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I252" s="1" t="s">
         <v>742</v>
@@ -10953,7 +10968,7 @@
         <v>15</v>
       </c>
       <c r="H253" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I253" s="1" t="s">
         <v>743</v>
@@ -10988,7 +11003,7 @@
         <v>15</v>
       </c>
       <c r="H254" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I254" s="1" t="s">
         <v>744</v>
@@ -11023,7 +11038,7 @@
         <v>15</v>
       </c>
       <c r="H255" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I255" s="1" t="s">
         <v>745</v>
@@ -11058,7 +11073,7 @@
         <v>15</v>
       </c>
       <c r="H256" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I256" s="1" t="s">
         <v>746</v>
@@ -11093,7 +11108,7 @@
         <v>15</v>
       </c>
       <c r="H257" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I257" s="1" t="s">
         <v>747</v>
@@ -11128,7 +11143,7 @@
         <v>15</v>
       </c>
       <c r="H258" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I258" s="1" t="s">
         <v>748</v>
@@ -11163,7 +11178,7 @@
         <v>15</v>
       </c>
       <c r="H259" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I259" s="1" t="s">
         <v>750</v>
@@ -11198,7 +11213,7 @@
         <v>15</v>
       </c>
       <c r="H260" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I260" s="1" t="s">
         <v>752</v>
@@ -11233,7 +11248,7 @@
         <v>15</v>
       </c>
       <c r="H261" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I261" s="1" t="s">
         <v>755</v>
@@ -11268,7 +11283,7 @@
         <v>15</v>
       </c>
       <c r="H262" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I262" s="1" t="s">
         <v>756</v>
@@ -11303,7 +11318,7 @@
         <v>15</v>
       </c>
       <c r="H263" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I263" s="1" t="s">
         <v>753</v>
@@ -11338,7 +11353,7 @@
         <v>15</v>
       </c>
       <c r="H264" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I264" s="1" t="s">
         <v>754</v>
@@ -11373,7 +11388,7 @@
         <v>15</v>
       </c>
       <c r="H265" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I265" s="1" t="s">
         <v>757</v>
@@ -11405,7 +11420,7 @@
         <v>15</v>
       </c>
       <c r="H266" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I266" s="1" t="s">
         <v>769</v>
@@ -11437,7 +11452,7 @@
         <v>15</v>
       </c>
       <c r="H267" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I267" s="1" t="s">
         <v>770</v>
@@ -11469,7 +11484,7 @@
         <v>15</v>
       </c>
       <c r="H268" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I268" s="1" t="s">
         <v>772</v>
@@ -11501,7 +11516,7 @@
         <v>15</v>
       </c>
       <c r="H269" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I269" s="1" t="s">
         <v>775</v>
@@ -11533,7 +11548,7 @@
         <v>15</v>
       </c>
       <c r="H270" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I270" s="1" t="s">
         <v>776</v>
@@ -11565,7 +11580,7 @@
         <v>15</v>
       </c>
       <c r="H271" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I271" s="1" t="s">
         <v>777</v>
@@ -11597,7 +11612,7 @@
         <v>15</v>
       </c>
       <c r="H272" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I272" s="1" t="s">
         <v>778</v>
@@ -11611,7 +11626,7 @@
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A273" s="1" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>25</v>
@@ -11643,7 +11658,7 @@
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A274" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>25</v>
@@ -11664,7 +11679,7 @@
         <v>786</v>
       </c>
       <c r="H274" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I274" s="1" t="s">
         <v>794</v>
@@ -11699,7 +11714,7 @@
         <v>786</v>
       </c>
       <c r="H275" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I275" s="1" t="s">
         <v>797</v>
@@ -11734,7 +11749,7 @@
         <v>786</v>
       </c>
       <c r="H276" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I276" s="1" t="s">
         <v>801</v>
@@ -11801,7 +11816,7 @@
         <v>786</v>
       </c>
       <c r="H278" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I278" s="1" t="s">
         <v>816</v>
@@ -11836,7 +11851,7 @@
         <v>786</v>
       </c>
       <c r="H279" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I279" s="1" t="s">
         <v>817</v>
@@ -11871,7 +11886,7 @@
         <v>786</v>
       </c>
       <c r="H280" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I280" s="1" t="s">
         <v>827</v>
@@ -11885,7 +11900,7 @@
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A281" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B281" s="1" t="s">
         <v>25</v>
@@ -11938,7 +11953,7 @@
         <v>826</v>
       </c>
       <c r="H282" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="I282" s="1" t="s">
         <v>833</v>
@@ -11973,7 +11988,7 @@
         <v>786</v>
       </c>
       <c r="H283" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I283" s="1" t="s">
         <v>836</v>
@@ -12008,7 +12023,7 @@
         <v>786</v>
       </c>
       <c r="H284" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I284" s="1" t="s">
         <v>849</v>
@@ -12043,7 +12058,7 @@
         <v>786</v>
       </c>
       <c r="H285" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I285" s="1" t="s">
         <v>850</v>
@@ -12078,7 +12093,7 @@
         <v>786</v>
       </c>
       <c r="H286" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I286" s="1" t="s">
         <v>851</v>
@@ -12113,7 +12128,7 @@
         <v>786</v>
       </c>
       <c r="H287" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I287" s="1" t="s">
         <v>852</v>
@@ -12148,7 +12163,7 @@
         <v>15</v>
       </c>
       <c r="H288" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I288" s="1" t="s">
         <v>900</v>
@@ -12183,7 +12198,7 @@
         <v>15</v>
       </c>
       <c r="H289" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I289" s="1" t="s">
         <v>901</v>
@@ -12218,7 +12233,7 @@
         <v>15</v>
       </c>
       <c r="H290" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I290" s="1" t="s">
         <v>902</v>
@@ -12253,7 +12268,7 @@
         <v>15</v>
       </c>
       <c r="H291" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I291" s="1" t="s">
         <v>903</v>
@@ -12288,7 +12303,7 @@
         <v>15</v>
       </c>
       <c r="H292" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I292" s="1" t="s">
         <v>904</v>
@@ -12323,7 +12338,7 @@
         <v>15</v>
       </c>
       <c r="H293" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I293" s="1" t="s">
         <v>905</v>
@@ -12358,7 +12373,7 @@
         <v>15</v>
       </c>
       <c r="H294" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I294" s="1" t="s">
         <v>906</v>
@@ -12393,7 +12408,7 @@
         <v>15</v>
       </c>
       <c r="H295" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I295" s="1" t="s">
         <v>907</v>
@@ -12428,7 +12443,7 @@
         <v>15</v>
       </c>
       <c r="H296" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I296" s="1" t="s">
         <v>908</v>
@@ -12463,7 +12478,7 @@
         <v>15</v>
       </c>
       <c r="H297" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I297" s="1" t="s">
         <v>909</v>
@@ -12498,7 +12513,7 @@
         <v>15</v>
       </c>
       <c r="H298" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I298" s="1" t="s">
         <v>910</v>
@@ -12533,7 +12548,7 @@
         <v>15</v>
       </c>
       <c r="H299" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I299" s="1" t="s">
         <v>911</v>
@@ -12568,7 +12583,7 @@
         <v>15</v>
       </c>
       <c r="H300" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I300" s="1" t="s">
         <v>912</v>
@@ -12603,7 +12618,7 @@
         <v>15</v>
       </c>
       <c r="H301" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I301" s="1" t="s">
         <v>913</v>
@@ -12638,7 +12653,7 @@
         <v>15</v>
       </c>
       <c r="H302" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I302" s="1" t="s">
         <v>914</v>
@@ -12673,7 +12688,7 @@
         <v>15</v>
       </c>
       <c r="H303" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I303" s="1" t="s">
         <v>915</v>
@@ -12708,7 +12723,7 @@
         <v>15</v>
       </c>
       <c r="H304" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I304" s="1" t="s">
         <v>916</v>
@@ -12743,7 +12758,7 @@
         <v>15</v>
       </c>
       <c r="H305" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I305" s="1" t="s">
         <v>917</v>
@@ -12778,7 +12793,7 @@
         <v>15</v>
       </c>
       <c r="H306" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I306" s="1" t="s">
         <v>920</v>
@@ -12813,7 +12828,7 @@
         <v>15</v>
       </c>
       <c r="H307" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I307" s="1" t="s">
         <v>922</v>
@@ -12874,7 +12889,7 @@
         <v>15</v>
       </c>
       <c r="H309" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I309" s="1" t="s">
         <v>928</v>
@@ -12909,7 +12924,7 @@
         <v>15</v>
       </c>
       <c r="H310" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I310" s="1" t="s">
         <v>930</v>
@@ -12938,7 +12953,7 @@
         <v>14</v>
       </c>
       <c r="H311" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I311" s="1" t="s">
         <v>941</v>
@@ -12967,7 +12982,7 @@
         <v>14</v>
       </c>
       <c r="H312" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I312" s="1" t="s">
         <v>943</v>
@@ -12996,7 +13011,7 @@
         <v>14</v>
       </c>
       <c r="H313" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I313" s="1" t="s">
         <v>946</v>
@@ -13025,7 +13040,7 @@
         <v>14</v>
       </c>
       <c r="H314" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I314" s="1" t="s">
         <v>949</v>
@@ -13039,7 +13054,7 @@
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A315" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B315" s="1" t="s">
         <v>25</v>
@@ -13080,7 +13095,7 @@
         <v>955</v>
       </c>
       <c r="H316" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="I316" s="1" t="s">
         <v>974</v>
@@ -13094,7 +13109,7 @@
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A317" s="1" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B317" s="1" t="s">
         <v>25</v>
@@ -13135,7 +13150,7 @@
         <v>959</v>
       </c>
       <c r="H318" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="I318" s="1" t="s">
         <v>962</v>
@@ -13164,7 +13179,7 @@
         <v>959</v>
       </c>
       <c r="H319" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="I319" s="1" t="s">
         <v>965</v>
@@ -13193,7 +13208,7 @@
         <v>14</v>
       </c>
       <c r="H320" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I320" s="1" t="s">
         <v>977</v>
@@ -13225,7 +13240,7 @@
         <v>15</v>
       </c>
       <c r="H321" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I321" s="1" t="s">
         <v>985</v>
@@ -13257,7 +13272,7 @@
         <v>15</v>
       </c>
       <c r="H322" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I322" s="1" t="s">
         <v>988</v>
@@ -13484,16 +13499,16 @@
         <v>25</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>951</v>
+        <v>1040</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>952</v>
+        <v>981</v>
       </c>
       <c r="I332" s="1" t="s">
-        <v>1022</v>
+        <v>1041</v>
       </c>
       <c r="J332" s="1" t="s">
-        <v>953</v>
+        <v>1042</v>
       </c>
       <c r="K332" s="1" t="s">
         <v>29</v>
@@ -13507,18 +13522,41 @@
         <v>25</v>
       </c>
       <c r="C333" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D333" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="I333" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J333" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="K333" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A334" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C334" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="D333" s="1" t="s">
+      <c r="D334" s="1" t="s">
         <v>1021</v>
       </c>
-      <c r="I333" s="1" t="s">
-        <v>1023</v>
-      </c>
-      <c r="J333" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="K333" s="1" t="s">
+      <c r="I334" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="J334" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="K334" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.6.0 final for tag
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5035" uniqueCount="1661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5037" uniqueCount="1661">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6144,12 +6144,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -6164,11 +6170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -6472,8 +6479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K564"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D537" workbookViewId="0">
-      <selection activeCell="I550" sqref="I550"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9477,6 +9484,9 @@
       <c r="A116" s="1" t="s">
         <v>306</v>
       </c>
+      <c r="B116" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C116" s="1" t="s">
         <v>347</v>
       </c>
@@ -9500,6 +9510,9 @@
       <c r="A117" s="1" t="s">
         <v>307</v>
       </c>
+      <c r="B117" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C117" s="1" t="s">
         <v>347</v>
       </c>
@@ -15833,7 +15846,7 @@
       </c>
     </row>
     <row r="336" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A336" s="1" t="s">
+      <c r="A336" s="4" t="s">
         <v>1062</v>
       </c>
       <c r="B336" s="1" t="s">
@@ -15862,7 +15875,7 @@
       </c>
     </row>
     <row r="337" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A337" s="1" t="s">
+      <c r="A337" s="4" t="s">
         <v>1048</v>
       </c>
       <c r="B337" s="1" t="s">
@@ -15894,7 +15907,7 @@
       </c>
     </row>
     <row r="338" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A338" s="1" t="s">
+      <c r="A338" s="4" t="s">
         <v>1049</v>
       </c>
       <c r="B338" s="1" t="s">
@@ -15926,7 +15939,7 @@
       </c>
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A339" s="1" t="s">
+      <c r="A339" s="4" t="s">
         <v>1050</v>
       </c>
       <c r="B339" s="1" t="s">
@@ -15958,7 +15971,7 @@
       </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A340" s="1" t="s">
+      <c r="A340" s="4" t="s">
         <v>1051</v>
       </c>
       <c r="B340" s="1" t="s">
@@ -15990,7 +16003,7 @@
       </c>
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A341" s="1" t="s">
+      <c r="A341" s="4" t="s">
         <v>1052</v>
       </c>
       <c r="B341" s="1" t="s">
@@ -16019,7 +16032,7 @@
       </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A342" s="1" t="s">
+      <c r="A342" s="4" t="s">
         <v>1053</v>
       </c>
       <c r="B342" s="1" t="s">
@@ -16051,7 +16064,7 @@
       </c>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A343" s="1" t="s">
+      <c r="A343" s="4" t="s">
         <v>1054</v>
       </c>
       <c r="B343" s="1" t="s">
@@ -16083,7 +16096,7 @@
       </c>
     </row>
     <row r="344" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A344" s="1" t="s">
+      <c r="A344" s="4" t="s">
         <v>1055</v>
       </c>
       <c r="B344" s="1" t="s">
@@ -16112,7 +16125,7 @@
       </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A345" s="1" t="s">
+      <c r="A345" s="4" t="s">
         <v>1056</v>
       </c>
       <c r="B345" s="1" t="s">
@@ -16144,7 +16157,7 @@
       </c>
     </row>
     <row r="346" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A346" s="1" t="s">
+      <c r="A346" s="4" t="s">
         <v>1057</v>
       </c>
       <c r="B346" s="1" t="s">
@@ -16176,7 +16189,7 @@
       </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A347" s="1" t="s">
+      <c r="A347" s="4" t="s">
         <v>1058</v>
       </c>
       <c r="B347" s="1" t="s">
@@ -16208,7 +16221,7 @@
       </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A348" s="1" t="s">
+      <c r="A348" s="4" t="s">
         <v>1059</v>
       </c>
       <c r="B348" s="1" t="s">
@@ -16237,7 +16250,7 @@
       </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A349" s="1" t="s">
+      <c r="A349" s="4" t="s">
         <v>1060</v>
       </c>
       <c r="B349" s="1" t="s">
@@ -16269,7 +16282,7 @@
       </c>
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A350" s="1" t="s">
+      <c r="A350" s="4" t="s">
         <v>1077</v>
       </c>
       <c r="B350" s="1" t="s">
@@ -16301,7 +16314,7 @@
       </c>
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A351" s="1" t="s">
+      <c r="A351" s="4" t="s">
         <v>1078</v>
       </c>
       <c r="B351" s="1" t="s">
@@ -16333,7 +16346,7 @@
       </c>
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A352" s="1" t="s">
+      <c r="A352" s="4" t="s">
         <v>1079</v>
       </c>
       <c r="B352" s="1" t="s">
@@ -16362,7 +16375,7 @@
       </c>
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A353" s="1" t="s">
+      <c r="A353" s="4" t="s">
         <v>1080</v>
       </c>
       <c r="B353" s="1" t="s">
@@ -16394,7 +16407,7 @@
       </c>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A354" s="1" t="s">
+      <c r="A354" s="4" t="s">
         <v>1081</v>
       </c>
       <c r="B354" s="1" t="s">
@@ -16426,7 +16439,7 @@
       </c>
     </row>
     <row r="355" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A355" s="1" t="s">
+      <c r="A355" s="4" t="s">
         <v>1082</v>
       </c>
       <c r="B355" s="1" t="s">
@@ -16455,7 +16468,7 @@
       </c>
     </row>
     <row r="356" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A356" s="1" t="s">
+      <c r="A356" s="4" t="s">
         <v>1083</v>
       </c>
       <c r="B356" s="1" t="s">
@@ -16487,7 +16500,7 @@
       </c>
     </row>
     <row r="357" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A357" s="1" t="s">
+      <c r="A357" s="4" t="s">
         <v>1084</v>
       </c>
       <c r="B357" s="1" t="s">
@@ -16519,7 +16532,7 @@
       </c>
     </row>
     <row r="358" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A358" s="1" t="s">
+      <c r="A358" s="4" t="s">
         <v>1085</v>
       </c>
       <c r="B358" s="1" t="s">
@@ -16551,7 +16564,7 @@
       </c>
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A359" s="1" t="s">
+      <c r="A359" s="4" t="s">
         <v>1086</v>
       </c>
       <c r="B359" s="1" t="s">
@@ -16583,7 +16596,7 @@
       </c>
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A360" s="1" t="s">
+      <c r="A360" s="4" t="s">
         <v>1087</v>
       </c>
       <c r="B360" s="1" t="s">
@@ -16612,7 +16625,7 @@
       </c>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A361" s="1" t="s">
+      <c r="A361" s="4" t="s">
         <v>1088</v>
       </c>
       <c r="B361" s="1" t="s">
@@ -16644,7 +16657,7 @@
       </c>
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A362" s="1" t="s">
+      <c r="A362" s="4" t="s">
         <v>1089</v>
       </c>
       <c r="B362" s="1" t="s">
@@ -16676,7 +16689,7 @@
       </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A363" s="1" t="s">
+      <c r="A363" s="4" t="s">
         <v>1112</v>
       </c>
       <c r="B363" s="1" t="s">
@@ -16708,7 +16721,7 @@
       </c>
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A364" s="1" t="s">
+      <c r="A364" s="4" t="s">
         <v>1113</v>
       </c>
       <c r="B364" s="1" t="s">
@@ -16740,7 +16753,7 @@
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A365" s="1" t="s">
+      <c r="A365" s="4" t="s">
         <v>1114</v>
       </c>
       <c r="B365" s="1" t="s">
@@ -16772,7 +16785,7 @@
       </c>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A366" s="1" t="s">
+      <c r="A366" s="4" t="s">
         <v>1115</v>
       </c>
       <c r="B366" s="1" t="s">
@@ -16804,7 +16817,7 @@
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A367" s="1" t="s">
+      <c r="A367" s="4" t="s">
         <v>1116</v>
       </c>
       <c r="B367" s="1" t="s">
@@ -16836,7 +16849,7 @@
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A368" s="1" t="s">
+      <c r="A368" s="4" t="s">
         <v>1117</v>
       </c>
       <c r="B368" s="1" t="s">
@@ -16868,7 +16881,7 @@
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A369" s="1" t="s">
+      <c r="A369" s="4" t="s">
         <v>1118</v>
       </c>
       <c r="B369" s="1" t="s">
@@ -16900,7 +16913,7 @@
       </c>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A370" s="1" t="s">
+      <c r="A370" s="4" t="s">
         <v>1119</v>
       </c>
       <c r="B370" s="1" t="s">
@@ -16932,7 +16945,7 @@
       </c>
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A371" s="1" t="s">
+      <c r="A371" s="4" t="s">
         <v>1120</v>
       </c>
       <c r="B371" s="1" t="s">
@@ -16964,7 +16977,7 @@
       </c>
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A372" s="1" t="s">
+      <c r="A372" s="4" t="s">
         <v>1121</v>
       </c>
       <c r="B372" s="1" t="s">
@@ -16996,7 +17009,7 @@
       </c>
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A373" s="1" t="s">
+      <c r="A373" s="4" t="s">
         <v>1122</v>
       </c>
       <c r="B373" s="1" t="s">
@@ -17028,7 +17041,7 @@
       </c>
     </row>
     <row r="374" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A374" s="1" t="s">
+      <c r="A374" s="4" t="s">
         <v>1123</v>
       </c>
       <c r="B374" s="1" t="s">
@@ -17060,7 +17073,7 @@
       </c>
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A375" s="1" t="s">
+      <c r="A375" s="4" t="s">
         <v>1124</v>
       </c>
       <c r="B375" s="1" t="s">
@@ -17092,7 +17105,7 @@
       </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A376" s="1" t="s">
+      <c r="A376" s="4" t="s">
         <v>1155</v>
       </c>
       <c r="B376" s="1" t="s">
@@ -17124,7 +17137,7 @@
       </c>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A377" s="1" t="s">
+      <c r="A377" s="4" t="s">
         <v>1156</v>
       </c>
       <c r="B377" s="1" t="s">
@@ -17156,7 +17169,7 @@
       </c>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A378" s="1" t="s">
+      <c r="A378" s="4" t="s">
         <v>1157</v>
       </c>
       <c r="B378" s="1" t="s">
@@ -17188,7 +17201,7 @@
       </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A379" s="1" t="s">
+      <c r="A379" s="4" t="s">
         <v>1158</v>
       </c>
       <c r="B379" s="1" t="s">
@@ -17220,7 +17233,7 @@
       </c>
     </row>
     <row r="380" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A380" s="1" t="s">
+      <c r="A380" s="4" t="s">
         <v>1159</v>
       </c>
       <c r="B380" s="1" t="s">
@@ -17252,7 +17265,7 @@
       </c>
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A381" s="1" t="s">
+      <c r="A381" s="4" t="s">
         <v>1160</v>
       </c>
       <c r="B381" s="1" t="s">
@@ -17284,7 +17297,7 @@
       </c>
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A382" s="1" t="s">
+      <c r="A382" s="4" t="s">
         <v>1161</v>
       </c>
       <c r="B382" s="1" t="s">
@@ -17316,7 +17329,7 @@
       </c>
     </row>
     <row r="383" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A383" s="1" t="s">
+      <c r="A383" s="4" t="s">
         <v>1162</v>
       </c>
       <c r="B383" s="1" t="s">
@@ -17348,7 +17361,7 @@
       </c>
     </row>
     <row r="384" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A384" s="1" t="s">
+      <c r="A384" s="4" t="s">
         <v>1163</v>
       </c>
       <c r="B384" s="1" t="s">
@@ -17380,7 +17393,7 @@
       </c>
     </row>
     <row r="385" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A385" s="1" t="s">
+      <c r="A385" s="4" t="s">
         <v>1164</v>
       </c>
       <c r="B385" s="1" t="s">
@@ -17412,7 +17425,7 @@
       </c>
     </row>
     <row r="386" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A386" s="1" t="s">
+      <c r="A386" s="4" t="s">
         <v>1165</v>
       </c>
       <c r="B386" s="1" t="s">
@@ -17444,7 +17457,7 @@
       </c>
     </row>
     <row r="387" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A387" s="1" t="s">
+      <c r="A387" s="4" t="s">
         <v>1166</v>
       </c>
       <c r="B387" s="1" t="s">
@@ -17476,7 +17489,7 @@
       </c>
     </row>
     <row r="388" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A388" s="1" t="s">
+      <c r="A388" s="4" t="s">
         <v>1167</v>
       </c>
       <c r="B388" s="1" t="s">
@@ -17508,7 +17521,7 @@
       </c>
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A389" s="1" t="s">
+      <c r="A389" s="4" t="s">
         <v>1187</v>
       </c>
       <c r="B389" s="1" t="s">
@@ -17540,7 +17553,7 @@
       </c>
     </row>
     <row r="390" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A390" s="1" t="s">
+      <c r="A390" s="4" t="s">
         <v>1188</v>
       </c>
       <c r="B390" s="1" t="s">
@@ -17572,7 +17585,7 @@
       </c>
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A391" s="1" t="s">
+      <c r="A391" s="4" t="s">
         <v>1189</v>
       </c>
       <c r="B391" s="1" t="s">
@@ -17604,7 +17617,7 @@
       </c>
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A392" s="1" t="s">
+      <c r="A392" s="4" t="s">
         <v>1190</v>
       </c>
       <c r="B392" s="1" t="s">
@@ -17636,7 +17649,7 @@
       </c>
     </row>
     <row r="393" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A393" s="1" t="s">
+      <c r="A393" s="4" t="s">
         <v>1191</v>
       </c>
       <c r="B393" s="1" t="s">
@@ -17668,7 +17681,7 @@
       </c>
     </row>
     <row r="394" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A394" s="1" t="s">
+      <c r="A394" s="4" t="s">
         <v>1192</v>
       </c>
       <c r="B394" s="1" t="s">
@@ -17700,7 +17713,7 @@
       </c>
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A395" s="1" t="s">
+      <c r="A395" s="4" t="s">
         <v>1193</v>
       </c>
       <c r="B395" s="1" t="s">
@@ -17732,7 +17745,7 @@
       </c>
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A396" s="1" t="s">
+      <c r="A396" s="4" t="s">
         <v>1194</v>
       </c>
       <c r="B396" s="1" t="s">
@@ -17764,7 +17777,7 @@
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A397" s="1" t="s">
+      <c r="A397" s="4" t="s">
         <v>1195</v>
       </c>
       <c r="B397" s="1" t="s">
@@ -17796,7 +17809,7 @@
       </c>
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A398" s="1" t="s">
+      <c r="A398" s="4" t="s">
         <v>1196</v>
       </c>
       <c r="B398" s="1" t="s">
@@ -17828,7 +17841,7 @@
       </c>
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A399" s="1" t="s">
+      <c r="A399" s="4" t="s">
         <v>1197</v>
       </c>
       <c r="B399" s="1" t="s">
@@ -17860,7 +17873,7 @@
       </c>
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A400" s="1" t="s">
+      <c r="A400" s="4" t="s">
         <v>1198</v>
       </c>
       <c r="B400" s="1" t="s">
@@ -17892,7 +17905,7 @@
       </c>
     </row>
     <row r="401" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A401" s="1" t="s">
+      <c r="A401" s="4" t="s">
         <v>1199</v>
       </c>
       <c r="B401" s="1" t="s">
@@ -17924,7 +17937,7 @@
       </c>
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A402" s="1" t="s">
+      <c r="A402" s="4" t="s">
         <v>1225</v>
       </c>
       <c r="B402" s="1" t="s">
@@ -17956,7 +17969,7 @@
       </c>
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A403" s="1" t="s">
+      <c r="A403" s="4" t="s">
         <v>1226</v>
       </c>
       <c r="B403" s="1" t="s">
@@ -17988,7 +18001,7 @@
       </c>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A404" s="1" t="s">
+      <c r="A404" s="4" t="s">
         <v>1227</v>
       </c>
       <c r="B404" s="1" t="s">
@@ -18020,7 +18033,7 @@
       </c>
     </row>
     <row r="405" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A405" s="1" t="s">
+      <c r="A405" s="4" t="s">
         <v>1228</v>
       </c>
       <c r="B405" s="1" t="s">
@@ -18052,7 +18065,7 @@
       </c>
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A406" s="1" t="s">
+      <c r="A406" s="4" t="s">
         <v>1229</v>
       </c>
       <c r="B406" s="1" t="s">
@@ -18084,7 +18097,7 @@
       </c>
     </row>
     <row r="407" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A407" s="1" t="s">
+      <c r="A407" s="4" t="s">
         <v>1230</v>
       </c>
       <c r="B407" s="1" t="s">
@@ -18116,7 +18129,7 @@
       </c>
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A408" s="1" t="s">
+      <c r="A408" s="4" t="s">
         <v>1231</v>
       </c>
       <c r="B408" s="1" t="s">
@@ -18148,7 +18161,7 @@
       </c>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A409" s="1" t="s">
+      <c r="A409" s="4" t="s">
         <v>1232</v>
       </c>
       <c r="B409" s="1" t="s">
@@ -18180,7 +18193,7 @@
       </c>
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A410" s="1" t="s">
+      <c r="A410" s="4" t="s">
         <v>1233</v>
       </c>
       <c r="B410" s="1" t="s">
@@ -18212,7 +18225,7 @@
       </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A411" s="1" t="s">
+      <c r="A411" s="4" t="s">
         <v>1234</v>
       </c>
       <c r="B411" s="1" t="s">
@@ -18244,7 +18257,7 @@
       </c>
     </row>
     <row r="412" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A412" s="1" t="s">
+      <c r="A412" s="4" t="s">
         <v>1235</v>
       </c>
       <c r="B412" s="1" t="s">
@@ -18276,7 +18289,7 @@
       </c>
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A413" s="1" t="s">
+      <c r="A413" s="4" t="s">
         <v>1236</v>
       </c>
       <c r="B413" s="1" t="s">
@@ -18308,7 +18321,7 @@
       </c>
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A414" s="1" t="s">
+      <c r="A414" s="4" t="s">
         <v>1237</v>
       </c>
       <c r="B414" s="1" t="s">
@@ -18340,7 +18353,7 @@
       </c>
     </row>
     <row r="415" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A415" s="1" t="s">
+      <c r="A415" s="4" t="s">
         <v>1238</v>
       </c>
       <c r="B415" s="1" t="s">
@@ -18372,7 +18385,7 @@
       </c>
     </row>
     <row r="416" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A416" s="1" t="s">
+      <c r="A416" s="4" t="s">
         <v>1239</v>
       </c>
       <c r="B416" s="1" t="s">
@@ -18404,7 +18417,7 @@
       </c>
     </row>
     <row r="417" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A417" s="1" t="s">
+      <c r="A417" s="4" t="s">
         <v>1240</v>
       </c>
       <c r="B417" s="1" t="s">
@@ -18436,7 +18449,7 @@
       </c>
     </row>
     <row r="418" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A418" s="1" t="s">
+      <c r="A418" s="4" t="s">
         <v>1241</v>
       </c>
       <c r="B418" s="1" t="s">
@@ -18468,7 +18481,7 @@
       </c>
     </row>
     <row r="419" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A419" s="1" t="s">
+      <c r="A419" s="4" t="s">
         <v>1242</v>
       </c>
       <c r="B419" s="1" t="s">
@@ -18500,7 +18513,7 @@
       </c>
     </row>
     <row r="420" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A420" s="1" t="s">
+      <c r="A420" s="4" t="s">
         <v>1243</v>
       </c>
       <c r="B420" s="1" t="s">
@@ -18532,7 +18545,7 @@
       </c>
     </row>
     <row r="421" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A421" s="1" t="s">
+      <c r="A421" s="4" t="s">
         <v>1244</v>
       </c>
       <c r="B421" s="1" t="s">
@@ -18564,7 +18577,7 @@
       </c>
     </row>
     <row r="422" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A422" s="1" t="s">
+      <c r="A422" s="4" t="s">
         <v>1245</v>
       </c>
       <c r="B422" s="1" t="s">
@@ -18596,7 +18609,7 @@
       </c>
     </row>
     <row r="423" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A423" s="1" t="s">
+      <c r="A423" s="4" t="s">
         <v>1246</v>
       </c>
       <c r="B423" s="1" t="s">
@@ -18628,7 +18641,7 @@
       </c>
     </row>
     <row r="424" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A424" s="1" t="s">
+      <c r="A424" s="4" t="s">
         <v>1247</v>
       </c>
       <c r="B424" s="1" t="s">
@@ -18660,7 +18673,7 @@
       </c>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A425" s="1" t="s">
+      <c r="A425" s="4" t="s">
         <v>1248</v>
       </c>
       <c r="B425" s="1" t="s">
@@ -18692,7 +18705,7 @@
       </c>
     </row>
     <row r="426" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A426" s="1" t="s">
+      <c r="A426" s="4" t="s">
         <v>1249</v>
       </c>
       <c r="B426" s="1" t="s">
@@ -18724,7 +18737,7 @@
       </c>
     </row>
     <row r="427" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A427" s="1" t="s">
+      <c r="A427" s="4" t="s">
         <v>1250</v>
       </c>
       <c r="B427" s="1" t="s">
@@ -18756,7 +18769,7 @@
       </c>
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A428" s="1" t="s">
+      <c r="A428" s="4" t="s">
         <v>1251</v>
       </c>
       <c r="B428" s="1" t="s">
@@ -18788,7 +18801,7 @@
       </c>
     </row>
     <row r="429" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A429" s="1" t="s">
+      <c r="A429" s="4" t="s">
         <v>1252</v>
       </c>
       <c r="B429" s="1" t="s">
@@ -18820,7 +18833,7 @@
       </c>
     </row>
     <row r="430" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A430" s="1" t="s">
+      <c r="A430" s="4" t="s">
         <v>1253</v>
       </c>
       <c r="B430" s="1" t="s">
@@ -18852,7 +18865,7 @@
       </c>
     </row>
     <row r="431" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A431" s="1" t="s">
+      <c r="A431" s="4" t="s">
         <v>1254</v>
       </c>
       <c r="B431" s="1" t="s">
@@ -18884,7 +18897,7 @@
       </c>
     </row>
     <row r="432" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A432" s="1" t="s">
+      <c r="A432" s="4" t="s">
         <v>1255</v>
       </c>
       <c r="B432" s="1" t="s">
@@ -18916,7 +18929,7 @@
       </c>
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A433" s="1" t="s">
+      <c r="A433" s="4" t="s">
         <v>1256</v>
       </c>
       <c r="B433" s="1" t="s">
@@ -18948,7 +18961,7 @@
       </c>
     </row>
     <row r="434" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A434" s="1" t="s">
+      <c r="A434" s="4" t="s">
         <v>1257</v>
       </c>
       <c r="B434" s="1" t="s">
@@ -18980,7 +18993,7 @@
       </c>
     </row>
     <row r="435" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A435" s="1" t="s">
+      <c r="A435" s="4" t="s">
         <v>1258</v>
       </c>
       <c r="B435" s="1" t="s">
@@ -19012,7 +19025,7 @@
       </c>
     </row>
     <row r="436" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A436" s="1" t="s">
+      <c r="A436" s="4" t="s">
         <v>1259</v>
       </c>
       <c r="B436" s="1" t="s">
@@ -19044,7 +19057,7 @@
       </c>
     </row>
     <row r="437" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A437" s="1" t="s">
+      <c r="A437" s="4" t="s">
         <v>1319</v>
       </c>
       <c r="B437" s="1" t="s">
@@ -19076,7 +19089,7 @@
       </c>
     </row>
     <row r="438" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A438" s="1" t="s">
+      <c r="A438" s="4" t="s">
         <v>1320</v>
       </c>
       <c r="B438" s="1" t="s">
@@ -19108,7 +19121,7 @@
       </c>
     </row>
     <row r="439" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A439" s="1" t="s">
+      <c r="A439" s="4" t="s">
         <v>1321</v>
       </c>
       <c r="B439" s="1" t="s">
@@ -19137,7 +19150,7 @@
       </c>
     </row>
     <row r="440" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A440" s="1" t="s">
+      <c r="A440" s="4" t="s">
         <v>1322</v>
       </c>
       <c r="B440" s="1" t="s">
@@ -19169,7 +19182,7 @@
       </c>
     </row>
     <row r="441" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A441" s="1" t="s">
+      <c r="A441" s="4" t="s">
         <v>1340</v>
       </c>
       <c r="B441" s="1" t="s">
@@ -19201,7 +19214,7 @@
       </c>
     </row>
     <row r="442" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A442" s="1" t="s">
+      <c r="A442" s="4" t="s">
         <v>1345</v>
       </c>
       <c r="B442" s="1" t="s">
@@ -19541,7 +19554,7 @@
       </c>
     </row>
     <row r="453" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A453" s="1" t="s">
+      <c r="A453" s="4" t="s">
         <v>1439</v>
       </c>
       <c r="B453" s="1" t="s">
@@ -19567,7 +19580,7 @@
       </c>
     </row>
     <row r="454" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A454" s="1" t="s">
+      <c r="A454" s="4" t="s">
         <v>1454</v>
       </c>
       <c r="B454" s="1" t="s">
@@ -19593,7 +19606,7 @@
       </c>
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A455" s="1" t="s">
+      <c r="A455" s="4" t="s">
         <v>1392</v>
       </c>
       <c r="B455" s="1" t="s">
@@ -19622,7 +19635,7 @@
       </c>
     </row>
     <row r="456" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A456" s="1" t="s">
+      <c r="A456" s="4" t="s">
         <v>1393</v>
       </c>
       <c r="B456" s="1" t="s">
@@ -19651,7 +19664,7 @@
       </c>
     </row>
     <row r="457" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A457" s="1" t="s">
+      <c r="A457" s="4" t="s">
         <v>1394</v>
       </c>
       <c r="B457" s="1" t="s">
@@ -19680,7 +19693,7 @@
       </c>
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A458" s="1" t="s">
+      <c r="A458" s="4" t="s">
         <v>1395</v>
       </c>
       <c r="B458" s="1" t="s">
@@ -19709,7 +19722,7 @@
       </c>
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A459" s="1" t="s">
+      <c r="A459" s="4" t="s">
         <v>1396</v>
       </c>
       <c r="B459" s="1" t="s">
@@ -19738,7 +19751,7 @@
       </c>
     </row>
     <row r="460" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A460" s="1" t="s">
+      <c r="A460" s="4" t="s">
         <v>1397</v>
       </c>
       <c r="B460" s="1" t="s">
@@ -19764,7 +19777,7 @@
       </c>
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A461" s="1" t="s">
+      <c r="A461" s="4" t="s">
         <v>1447</v>
       </c>
       <c r="B461" s="1" t="s">
@@ -19793,7 +19806,7 @@
       </c>
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A462" s="1" t="s">
+      <c r="A462" s="4" t="s">
         <v>1398</v>
       </c>
       <c r="B462" s="1" t="s">
@@ -19822,7 +19835,7 @@
       </c>
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A463" s="1" t="s">
+      <c r="A463" s="4" t="s">
         <v>1399</v>
       </c>
       <c r="B463" s="1" t="s">
@@ -19851,7 +19864,7 @@
       </c>
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A464" s="1" t="s">
+      <c r="A464" s="4" t="s">
         <v>1400</v>
       </c>
       <c r="B464" s="1" t="s">
@@ -19880,7 +19893,7 @@
       </c>
     </row>
     <row r="465" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A465" s="1" t="s">
+      <c r="A465" s="4" t="s">
         <v>1401</v>
       </c>
       <c r="B465" s="1" t="s">
@@ -19909,7 +19922,7 @@
       </c>
     </row>
     <row r="466" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A466" s="1" t="s">
+      <c r="A466" s="4" t="s">
         <v>1402</v>
       </c>
       <c r="B466" s="1" t="s">
@@ -19938,7 +19951,7 @@
       </c>
     </row>
     <row r="467" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A467" s="1" t="s">
+      <c r="A467" s="4" t="s">
         <v>1403</v>
       </c>
       <c r="B467" s="1" t="s">
@@ -19967,7 +19980,7 @@
       </c>
     </row>
     <row r="468" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A468" s="1" t="s">
+      <c r="A468" s="4" t="s">
         <v>1462</v>
       </c>
       <c r="B468" s="1" t="s">
@@ -19993,7 +20006,7 @@
       </c>
     </row>
     <row r="469" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A469" s="1" t="s">
+      <c r="A469" s="4" t="s">
         <v>1404</v>
       </c>
       <c r="B469" s="1" t="s">
@@ -20022,7 +20035,7 @@
       </c>
     </row>
     <row r="470" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A470" s="1" t="s">
+      <c r="A470" s="4" t="s">
         <v>1405</v>
       </c>
       <c r="B470" s="1" t="s">
@@ -20051,7 +20064,7 @@
       </c>
     </row>
     <row r="471" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A471" s="1" t="s">
+      <c r="A471" s="4" t="s">
         <v>1406</v>
       </c>
       <c r="B471" s="1" t="s">
@@ -20080,7 +20093,7 @@
       </c>
     </row>
     <row r="472" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A472" s="1" t="s">
+      <c r="A472" s="4" t="s">
         <v>1407</v>
       </c>
       <c r="B472" s="1" t="s">
@@ -20109,7 +20122,7 @@
       </c>
     </row>
     <row r="473" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A473" s="1" t="s">
+      <c r="A473" s="4" t="s">
         <v>1408</v>
       </c>
       <c r="B473" s="1" t="s">
@@ -20138,7 +20151,7 @@
       </c>
     </row>
     <row r="474" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A474" s="1" t="s">
+      <c r="A474" s="4" t="s">
         <v>1409</v>
       </c>
       <c r="B474" s="1" t="s">
@@ -20167,7 +20180,7 @@
       </c>
     </row>
     <row r="475" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A475" s="1" t="s">
+      <c r="A475" s="4" t="s">
         <v>1410</v>
       </c>
       <c r="B475" s="1" t="s">
@@ -20196,7 +20209,7 @@
       </c>
     </row>
     <row r="476" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A476" s="1" t="s">
+      <c r="A476" s="4" t="s">
         <v>1411</v>
       </c>
       <c r="B476" s="1" t="s">
@@ -20225,7 +20238,7 @@
       </c>
     </row>
     <row r="477" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A477" s="1" t="s">
+      <c r="A477" s="4" t="s">
         <v>1412</v>
       </c>
       <c r="B477" s="1" t="s">
@@ -20254,7 +20267,7 @@
       </c>
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A478" s="1" t="s">
+      <c r="A478" s="4" t="s">
         <v>1413</v>
       </c>
       <c r="B478" s="1" t="s">
@@ -20283,7 +20296,7 @@
       </c>
     </row>
     <row r="479" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A479" s="1" t="s">
+      <c r="A479" s="4" t="s">
         <v>1414</v>
       </c>
       <c r="B479" s="1" t="s">
@@ -20312,7 +20325,7 @@
       </c>
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A480" s="1" t="s">
+      <c r="A480" s="4" t="s">
         <v>1477</v>
       </c>
       <c r="B480" s="1" t="s">
@@ -20338,7 +20351,7 @@
       </c>
     </row>
     <row r="481" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A481" s="1" t="s">
+      <c r="A481" s="4" t="s">
         <v>1415</v>
       </c>
       <c r="B481" s="1" t="s">
@@ -20367,7 +20380,7 @@
       </c>
     </row>
     <row r="482" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A482" s="1" t="s">
+      <c r="A482" s="4" t="s">
         <v>1416</v>
       </c>
       <c r="B482" s="1" t="s">
@@ -20396,7 +20409,7 @@
       </c>
     </row>
     <row r="483" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A483" s="1" t="s">
+      <c r="A483" s="4" t="s">
         <v>1417</v>
       </c>
       <c r="B483" s="1" t="s">
@@ -20425,7 +20438,7 @@
       </c>
     </row>
     <row r="484" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A484" s="1" t="s">
+      <c r="A484" s="4" t="s">
         <v>1418</v>
       </c>
       <c r="B484" s="1" t="s">
@@ -20454,7 +20467,7 @@
       </c>
     </row>
     <row r="485" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A485" s="1" t="s">
+      <c r="A485" s="4" t="s">
         <v>1419</v>
       </c>
       <c r="B485" s="1" t="s">
@@ -20483,7 +20496,7 @@
       </c>
     </row>
     <row r="486" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A486" s="1" t="s">
+      <c r="A486" s="4" t="s">
         <v>1420</v>
       </c>
       <c r="B486" s="1" t="s">
@@ -20512,7 +20525,7 @@
       </c>
     </row>
     <row r="487" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A487" s="1" t="s">
+      <c r="A487" s="4" t="s">
         <v>1421</v>
       </c>
       <c r="B487" s="1" t="s">
@@ -20541,7 +20554,7 @@
       </c>
     </row>
     <row r="488" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A488" s="1" t="s">
+      <c r="A488" s="4" t="s">
         <v>1422</v>
       </c>
       <c r="B488" s="1" t="s">
@@ -20570,7 +20583,7 @@
       </c>
     </row>
     <row r="489" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A489" s="1" t="s">
+      <c r="A489" s="4" t="s">
         <v>1423</v>
       </c>
       <c r="B489" s="1" t="s">
@@ -20599,7 +20612,7 @@
       </c>
     </row>
     <row r="490" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A490" s="1" t="s">
+      <c r="A490" s="4" t="s">
         <v>1424</v>
       </c>
       <c r="B490" s="1" t="s">
@@ -20628,7 +20641,7 @@
       </c>
     </row>
     <row r="491" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A491" s="1" t="s">
+      <c r="A491" s="4" t="s">
         <v>1425</v>
       </c>
       <c r="B491" s="1" t="s">
@@ -20657,7 +20670,7 @@
       </c>
     </row>
     <row r="492" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A492" s="1" t="s">
+      <c r="A492" s="4" t="s">
         <v>1426</v>
       </c>
       <c r="B492" s="1" t="s">
@@ -20686,7 +20699,7 @@
       </c>
     </row>
     <row r="493" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A493" s="1" t="s">
+      <c r="A493" s="4" t="s">
         <v>1500</v>
       </c>
       <c r="B493" s="1" t="s">
@@ -20712,7 +20725,7 @@
       </c>
     </row>
     <row r="494" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A494" s="1" t="s">
+      <c r="A494" s="4" t="s">
         <v>1427</v>
       </c>
       <c r="B494" s="1" t="s">
@@ -20741,7 +20754,7 @@
       </c>
     </row>
     <row r="495" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A495" s="1" t="s">
+      <c r="A495" s="4" t="s">
         <v>1428</v>
       </c>
       <c r="B495" s="1" t="s">
@@ -20770,7 +20783,7 @@
       </c>
     </row>
     <row r="496" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A496" s="1" t="s">
+      <c r="A496" s="4" t="s">
         <v>1429</v>
       </c>
       <c r="B496" s="1" t="s">
@@ -20799,7 +20812,7 @@
       </c>
     </row>
     <row r="497" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A497" s="1" t="s">
+      <c r="A497" s="4" t="s">
         <v>1430</v>
       </c>
       <c r="B497" s="1" t="s">
@@ -20828,7 +20841,7 @@
       </c>
     </row>
     <row r="498" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A498" s="1" t="s">
+      <c r="A498" s="4" t="s">
         <v>1431</v>
       </c>
       <c r="B498" s="1" t="s">
@@ -20857,7 +20870,7 @@
       </c>
     </row>
     <row r="499" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A499" s="1" t="s">
+      <c r="A499" s="4" t="s">
         <v>1432</v>
       </c>
       <c r="B499" s="1" t="s">
@@ -20886,7 +20899,7 @@
       </c>
     </row>
     <row r="500" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A500" s="1" t="s">
+      <c r="A500" s="4" t="s">
         <v>1433</v>
       </c>
       <c r="B500" s="1" t="s">
@@ -20915,7 +20928,7 @@
       </c>
     </row>
     <row r="501" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A501" s="1" t="s">
+      <c r="A501" s="4" t="s">
         <v>1492</v>
       </c>
       <c r="B501" s="1" t="s">
@@ -20944,7 +20957,7 @@
       </c>
     </row>
     <row r="502" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A502" s="1" t="s">
+      <c r="A502" s="4" t="s">
         <v>1493</v>
       </c>
       <c r="B502" s="1" t="s">
@@ -20973,7 +20986,7 @@
       </c>
     </row>
     <row r="503" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A503" s="1" t="s">
+      <c r="A503" s="4" t="s">
         <v>1494</v>
       </c>
       <c r="B503" s="1" t="s">
@@ -21002,7 +21015,7 @@
       </c>
     </row>
     <row r="504" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A504" s="1" t="s">
+      <c r="A504" s="4" t="s">
         <v>1495</v>
       </c>
       <c r="B504" s="1" t="s">
@@ -21031,7 +21044,7 @@
       </c>
     </row>
     <row r="505" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A505" s="1" t="s">
+      <c r="A505" s="4" t="s">
         <v>1496</v>
       </c>
       <c r="B505" s="1" t="s">
@@ -21060,7 +21073,7 @@
       </c>
     </row>
     <row r="506" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A506" s="1" t="s">
+      <c r="A506" s="4" t="s">
         <v>1497</v>
       </c>
       <c r="B506" s="1" t="s">
@@ -21089,7 +21102,7 @@
       </c>
     </row>
     <row r="507" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A507" s="1" t="s">
+      <c r="A507" s="4" t="s">
         <v>1498</v>
       </c>
       <c r="B507" s="1" t="s">
@@ -21118,7 +21131,7 @@
       </c>
     </row>
     <row r="508" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A508" s="1" t="s">
+      <c r="A508" s="4" t="s">
         <v>1499</v>
       </c>
       <c r="B508" s="1" t="s">
@@ -21147,7 +21160,7 @@
       </c>
     </row>
     <row r="509" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A509" s="1" t="s">
+      <c r="A509" s="4" t="s">
         <v>1524</v>
       </c>
       <c r="B509" s="1" t="s">
@@ -21176,7 +21189,7 @@
       </c>
     </row>
     <row r="510" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A510" s="1" t="s">
+      <c r="A510" s="4" t="s">
         <v>1535</v>
       </c>
       <c r="B510" s="1" t="s">
@@ -21202,7 +21215,7 @@
       </c>
     </row>
     <row r="511" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A511" s="1" t="s">
+      <c r="A511" s="4" t="s">
         <v>1525</v>
       </c>
       <c r="B511" s="1" t="s">
@@ -21231,7 +21244,7 @@
       </c>
     </row>
     <row r="512" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A512" s="1" t="s">
+      <c r="A512" s="4" t="s">
         <v>1526</v>
       </c>
       <c r="B512" s="1" t="s">
@@ -21260,7 +21273,7 @@
       </c>
     </row>
     <row r="513" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A513" s="1" t="s">
+      <c r="A513" s="4" t="s">
         <v>1527</v>
       </c>
       <c r="B513" s="1" t="s">
@@ -21289,7 +21302,7 @@
       </c>
     </row>
     <row r="514" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A514" s="1" t="s">
+      <c r="A514" s="4" t="s">
         <v>1528</v>
       </c>
       <c r="B514" s="1" t="s">
@@ -21318,7 +21331,7 @@
       </c>
     </row>
     <row r="515" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A515" s="1" t="s">
+      <c r="A515" s="4" t="s">
         <v>1529</v>
       </c>
       <c r="B515" s="1" t="s">
@@ -21347,7 +21360,7 @@
       </c>
     </row>
     <row r="516" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A516" s="1" t="s">
+      <c r="A516" s="4" t="s">
         <v>1530</v>
       </c>
       <c r="B516" s="1" t="s">
@@ -21376,7 +21389,7 @@
       </c>
     </row>
     <row r="517" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A517" s="1" t="s">
+      <c r="A517" s="4" t="s">
         <v>1543</v>
       </c>
       <c r="B517" s="1" t="s">
@@ -21405,7 +21418,7 @@
       </c>
     </row>
     <row r="518" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A518" s="1" t="s">
+      <c r="A518" s="4" t="s">
         <v>1544</v>
       </c>
       <c r="B518" s="1" t="s">
@@ -21434,7 +21447,7 @@
       </c>
     </row>
     <row r="519" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A519" s="1" t="s">
+      <c r="A519" s="4" t="s">
         <v>1545</v>
       </c>
       <c r="B519" s="1" t="s">
@@ -21463,7 +21476,7 @@
       </c>
     </row>
     <row r="520" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A520" s="1" t="s">
+      <c r="A520" s="4" t="s">
         <v>1546</v>
       </c>
       <c r="B520" s="1" t="s">
@@ -21492,7 +21505,7 @@
       </c>
     </row>
     <row r="521" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A521" s="1" t="s">
+      <c r="A521" s="4" t="s">
         <v>1547</v>
       </c>
       <c r="B521" s="1" t="s">
@@ -21521,7 +21534,7 @@
       </c>
     </row>
     <row r="522" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A522" s="1" t="s">
+      <c r="A522" s="4" t="s">
         <v>1548</v>
       </c>
       <c r="B522" s="1" t="s">
@@ -21550,7 +21563,7 @@
       </c>
     </row>
     <row r="523" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A523" s="1" t="s">
+      <c r="A523" s="4" t="s">
         <v>1549</v>
       </c>
       <c r="B523" s="1" t="s">
@@ -21579,7 +21592,7 @@
       </c>
     </row>
     <row r="524" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A524" s="1" t="s">
+      <c r="A524" s="4" t="s">
         <v>1550</v>
       </c>
       <c r="B524" s="1" t="s">
@@ -21608,7 +21621,7 @@
       </c>
     </row>
     <row r="525" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A525" s="1" t="s">
+      <c r="A525" s="4" t="s">
         <v>1551</v>
       </c>
       <c r="B525" s="1" t="s">
@@ -21637,7 +21650,7 @@
       </c>
     </row>
     <row r="526" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A526" s="1" t="s">
+      <c r="A526" s="4" t="s">
         <v>1552</v>
       </c>
       <c r="B526" s="1" t="s">
@@ -21666,7 +21679,7 @@
       </c>
     </row>
     <row r="527" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A527" s="1" t="s">
+      <c r="A527" s="4" t="s">
         <v>1553</v>
       </c>
       <c r="B527" s="1" t="s">
@@ -21695,7 +21708,7 @@
       </c>
     </row>
     <row r="528" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A528" s="1" t="s">
+      <c r="A528" s="4" t="s">
         <v>1554</v>
       </c>
       <c r="B528" s="1" t="s">
@@ -21724,7 +21737,7 @@
       </c>
     </row>
     <row r="529" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A529" s="1" t="s">
+      <c r="A529" s="4" t="s">
         <v>1565</v>
       </c>
       <c r="B529" s="1" t="s">
@@ -21753,7 +21766,7 @@
       </c>
     </row>
     <row r="530" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A530" s="1" t="s">
+      <c r="A530" s="4" t="s">
         <v>1566</v>
       </c>
       <c r="B530" s="1" t="s">
@@ -21782,7 +21795,7 @@
       </c>
     </row>
     <row r="531" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A531" s="1" t="s">
+      <c r="A531" s="4" t="s">
         <v>1567</v>
       </c>
       <c r="B531" s="1" t="s">
@@ -21811,7 +21824,7 @@
       </c>
     </row>
     <row r="532" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A532" s="1" t="s">
+      <c r="A532" s="4" t="s">
         <v>1568</v>
       </c>
       <c r="B532" s="1" t="s">
@@ -21840,7 +21853,7 @@
       </c>
     </row>
     <row r="533" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A533" s="1" t="s">
+      <c r="A533" s="4" t="s">
         <v>1580</v>
       </c>
       <c r="B533" s="1" t="s">
@@ -21869,7 +21882,7 @@
       </c>
     </row>
     <row r="534" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A534" s="1" t="s">
+      <c r="A534" s="4" t="s">
         <v>1581</v>
       </c>
       <c r="B534" s="1" t="s">
@@ -21898,7 +21911,7 @@
       </c>
     </row>
     <row r="535" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A535" s="1" t="s">
+      <c r="A535" s="4" t="s">
         <v>1582</v>
       </c>
       <c r="B535" s="1" t="s">
@@ -21927,7 +21940,7 @@
       </c>
     </row>
     <row r="536" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A536" s="1" t="s">
+      <c r="A536" s="4" t="s">
         <v>1583</v>
       </c>
       <c r="B536" s="1" t="s">
@@ -21956,7 +21969,7 @@
       </c>
     </row>
     <row r="537" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A537" s="1" t="s">
+      <c r="A537" s="4" t="s">
         <v>1584</v>
       </c>
       <c r="B537" s="1" t="s">
@@ -21985,7 +21998,7 @@
       </c>
     </row>
     <row r="538" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A538" s="1" t="s">
+      <c r="A538" s="4" t="s">
         <v>1585</v>
       </c>
       <c r="B538" s="1" t="s">
@@ -22014,7 +22027,7 @@
       </c>
     </row>
     <row r="539" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A539" s="1" t="s">
+      <c r="A539" s="4" t="s">
         <v>1586</v>
       </c>
       <c r="B539" s="1" t="s">
@@ -22043,7 +22056,7 @@
       </c>
     </row>
     <row r="540" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A540" s="1" t="s">
+      <c r="A540" s="4" t="s">
         <v>1587</v>
       </c>
       <c r="B540" s="1" t="s">
@@ -22072,7 +22085,7 @@
       </c>
     </row>
     <row r="541" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A541" s="1" t="s">
+      <c r="A541" s="4" t="s">
         <v>1590</v>
       </c>
       <c r="B541" s="1" t="s">
@@ -22101,7 +22114,7 @@
       </c>
     </row>
     <row r="542" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A542" s="1" t="s">
+      <c r="A542" s="4" t="s">
         <v>1591</v>
       </c>
       <c r="B542" s="1" t="s">
@@ -22130,7 +22143,7 @@
       </c>
     </row>
     <row r="543" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A543" s="1" t="s">
+      <c r="A543" s="4" t="s">
         <v>1592</v>
       </c>
       <c r="B543" s="1" t="s">
@@ -22159,7 +22172,7 @@
       </c>
     </row>
     <row r="544" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A544" s="1" t="s">
+      <c r="A544" s="4" t="s">
         <v>1593</v>
       </c>
       <c r="B544" s="1" t="s">
@@ -22188,7 +22201,7 @@
       </c>
     </row>
     <row r="545" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A545" s="1" t="s">
+      <c r="A545" s="4" t="s">
         <v>1594</v>
       </c>
       <c r="B545" s="1" t="s">
@@ -22217,7 +22230,7 @@
       </c>
     </row>
     <row r="546" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A546" s="1" t="s">
+      <c r="A546" s="4" t="s">
         <v>1595</v>
       </c>
       <c r="B546" s="1" t="s">
@@ -22246,7 +22259,7 @@
       </c>
     </row>
     <row r="547" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A547" s="1" t="s">
+      <c r="A547" s="4" t="s">
         <v>1596</v>
       </c>
       <c r="B547" s="1" t="s">
@@ -22275,7 +22288,7 @@
       </c>
     </row>
     <row r="548" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A548" s="1" t="s">
+      <c r="A548" s="4" t="s">
         <v>1598</v>
       </c>
       <c r="B548" s="1" t="s">
@@ -22304,7 +22317,7 @@
       </c>
     </row>
     <row r="549" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A549" s="1" t="s">
+      <c r="A549" s="4" t="s">
         <v>1599</v>
       </c>
       <c r="B549" s="1" t="s">
@@ -22333,7 +22346,7 @@
       </c>
     </row>
     <row r="550" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A550" s="1" t="s">
+      <c r="A550" s="4" t="s">
         <v>1600</v>
       </c>
       <c r="B550" s="1" t="s">
@@ -22362,7 +22375,7 @@
       </c>
     </row>
     <row r="551" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A551" s="1" t="s">
+      <c r="A551" s="4" t="s">
         <v>1601</v>
       </c>
       <c r="B551" s="1" t="s">
@@ -22391,7 +22404,7 @@
       </c>
     </row>
     <row r="552" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A552" s="1" t="s">
+      <c r="A552" s="4" t="s">
         <v>1602</v>
       </c>
       <c r="B552" s="1" t="s">
@@ -22420,7 +22433,7 @@
       </c>
     </row>
     <row r="553" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A553" s="1" t="s">
+      <c r="A553" s="4" t="s">
         <v>1603</v>
       </c>
       <c r="B553" s="1" t="s">
@@ -22449,7 +22462,7 @@
       </c>
     </row>
     <row r="554" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A554" s="1" t="s">
+      <c r="A554" s="4" t="s">
         <v>1625</v>
       </c>
       <c r="B554" s="1" t="s">
@@ -22478,7 +22491,7 @@
       </c>
     </row>
     <row r="555" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A555" s="1" t="s">
+      <c r="A555" s="4" t="s">
         <v>1626</v>
       </c>
       <c r="B555" s="1" t="s">
@@ -22507,7 +22520,7 @@
       </c>
     </row>
     <row r="556" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A556" s="1" t="s">
+      <c r="A556" s="4" t="s">
         <v>1627</v>
       </c>
       <c r="B556" s="1" t="s">
@@ -22536,7 +22549,7 @@
       </c>
     </row>
     <row r="557" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A557" s="1" t="s">
+      <c r="A557" s="4" t="s">
         <v>1635</v>
       </c>
       <c r="B557" s="1" t="s">
@@ -22562,7 +22575,7 @@
       </c>
     </row>
     <row r="558" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A558" s="1" t="s">
+      <c r="A558" s="4" t="s">
         <v>1628</v>
       </c>
       <c r="B558" s="1" t="s">
@@ -22591,7 +22604,7 @@
       </c>
     </row>
     <row r="559" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A559" s="1" t="s">
+      <c r="A559" s="4" t="s">
         <v>1638</v>
       </c>
       <c r="B559" s="1" t="s">
@@ -22620,7 +22633,7 @@
       </c>
     </row>
     <row r="560" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A560" s="1" t="s">
+      <c r="A560" s="4" t="s">
         <v>1644</v>
       </c>
       <c r="B560" s="1" t="s">

</xml_diff>

<commit_message>
add scalar case about overlap index
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5091" uniqueCount="1692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5103" uniqueCount="1697">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6289,6 +6289,40 @@
   </si>
   <si>
     <t>ERROR 9001 (45000): Partition values count must be &lt;= key columns count, but values count is 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_572</t>
+  </si>
+  <si>
+    <t>三节点集群，索引副本数4，创建失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): Not enough regions is created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table neg_572 (
+    id bigint,
+    name varchar(32),
+    age int,
+    gmt bigint,
+    price FLOAT,
+    amount DOUBLE,
+    address varchar(255),
+    birthday DATE,
+    create_time TIME,
+    update_time TIMESTAMP,
+    zip_code varchar(20),
+    is_delete boolean,
+    PRIMARY KEY (id,name,birthday),
+    index age_index (age) replica=4
+)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6657,10 +6691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K572"/>
+  <dimension ref="A1:K573"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D571" workbookViewId="0">
-      <selection activeCell="I571" sqref="I571"/>
+    <sheetView tabSelected="1" topLeftCell="D572" workbookViewId="0">
+      <selection activeCell="H573" sqref="H573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -23017,6 +23051,9 @@
       <c r="D569" s="1" t="s">
         <v>981</v>
       </c>
+      <c r="E569" s="1" t="s">
+        <v>1694</v>
+      </c>
       <c r="I569" s="5" t="s">
         <v>1677</v>
       </c>
@@ -23040,6 +23077,9 @@
       <c r="D570" s="1" t="s">
         <v>981</v>
       </c>
+      <c r="E570" s="1" t="s">
+        <v>1694</v>
+      </c>
       <c r="I570" s="5" t="s">
         <v>1682</v>
       </c>
@@ -23063,6 +23103,9 @@
       <c r="D571" s="1" t="s">
         <v>981</v>
       </c>
+      <c r="E571" s="1" t="s">
+        <v>1694</v>
+      </c>
       <c r="I571" s="5" t="s">
         <v>1686</v>
       </c>
@@ -23086,6 +23129,9 @@
       <c r="D572" s="1" t="s">
         <v>981</v>
       </c>
+      <c r="E572" s="1" t="s">
+        <v>1694</v>
+      </c>
       <c r="I572" s="5" t="s">
         <v>1690</v>
       </c>
@@ -23093,6 +23139,32 @@
         <v>1691</v>
       </c>
       <c r="K572" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="573" spans="1:11" ht="216" x14ac:dyDescent="0.15">
+      <c r="A573" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B573" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C573" s="1" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D573" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="E573" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="I573" s="5" t="s">
+        <v>1696</v>
+      </c>
+      <c r="J573" s="1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="K573" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update nbits_per_idx param name
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5236" uniqueCount="1761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5362" uniqueCount="1820">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6553,6 +6553,403 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ERROR 9001 (45000): ivf_pq_parameter vector_index_parameter is illegal, dimension:64 / nsubvector:5 not divisible</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(2,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', '0')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(3,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', '1')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(4,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 'true')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(5,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 'False')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(6,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', true1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(7,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', isFalse)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(8,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', isTrue)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(9,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', False0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(10,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07',-2.5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(11,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07',1.4)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(12,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 0.5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(13,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 0.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>布尔字段类型名称为bool，创建表失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(1,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(2,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 1, true)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema1 values(3,'zhangsan','abc',23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07',true)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema7 values(2,'Li Si','male','1998-03-15',null,5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $array10 values(407,'zhangsan',18,23.5,array[2.5])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_590</t>
+  </si>
+  <si>
+    <t>negative_591</t>
+  </si>
+  <si>
+    <t>negative_592</t>
+  </si>
+  <si>
+    <t>向量topK查询，K缺失</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量topK查询，K为字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量topK查询，K为负整数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量topK查询，K大于1024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector001_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector001, feature, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): Incorrect parameter count for vector function.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_589</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_589</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector001, feature, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784], 'a')</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): Top n not number.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector001, feature, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784], -1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 5001 (45000): io.dingodb.sdk.common.DingoClientException$RequestErrorException: Param top_n 4294967295 is exceed max batch count 1024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector001, feature, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784], 1025)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 5001 (45000): io.dingodb.sdk.common.DingoClientException$RequestErrorException: Param top_n 1025 is exceed max batch count 1024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_593</t>
+  </si>
+  <si>
+    <t>negative_594</t>
+  </si>
+  <si>
+    <t>negative_595</t>
+  </si>
+  <si>
+    <t>创建IVFFlat算法的索引表，缺少ncentroids参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table neg_593 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfflat, metricType=L2, dimension=8),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): ivf_flat_parameter.ncentroids is illegal : 0  default : 2048</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建IVFFlat算法的索引表，ncentroids参数为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table neg_594 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfflat, metricType=L2, dimension=8, ncentroids=0),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_596</t>
+  </si>
+  <si>
+    <t>创建IVFFlat算法的索引表，ncentroids参数为小数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建IVFFlat算法的索引表，ncentroids参数为负数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table neg_595 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfflat, metricType=L2, dimension=8, ncentroids=2.5),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 3001 (45000): For input string: "2.5"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create table neg_596 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfflat, metricType=L2, dimension=8, ncentroids=-8),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_597</t>
+  </si>
+  <si>
+    <t>negative_598</t>
+  </si>
+  <si>
+    <t>创建IVFPQ算法的索引表，nbitsPerIdx为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE neg_597 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=16, ncentroids=10, nsubvector=4, nbitsPerIdx=0),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): ivf_pq_parameter.nbits_per_idx is illegal : 0 nbits_per_idx valid : (0, 16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建IVFPQ算法的索引表，nbitsPerIdx大于16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE neg_598 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=16, ncentroids=10, nsubvector=4, nbitsPerIdx=17),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): ivf_pq_parameter.nbits_per_idx is illegal : 17 nbits_per_idx valid : (0, 16]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_599</t>
+  </si>
+  <si>
+    <t>CREATE TABLE neg_599 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=16, ncentroids=10, nsubvector=4, nbitsPerIdx=-1),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建IVFPQ算法的索引表，nbitsPerIdx负数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建IVFPQ算法的索引表，nsubvector为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_600</t>
+  </si>
+  <si>
+    <t>CREATE TABLE neg_600 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=16, ncentroids=10, nsubvector=0, nbitsPerIdx=4),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): ivf_pq_parameter.nsubvector is illegal : 0 default : 64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_601</t>
+  </si>
+  <si>
+    <t>创建IVFPQ算法的索引表，dimension为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE neg_601 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=0, ncentroids=10, nsubvector=4, nbitsPerIdx=4),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): ivf_pq_parameter.dimension is illegal 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE neg_602 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=0, ncentroids=10, nsubvector=0, nbitsPerIdx=4),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建IVFPQ算法的索引表，dimension为0, nsubvctor也为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>negative_602</t>
+  </si>
+  <si>
+    <t>negative_603</t>
+  </si>
+  <si>
+    <t>创建IVFPQ算法的索引表，ncentroids为0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CREATE TABLE neg_603 (
+    id bigint auto_increment not null, 
+    name varchar(32),
+    age int,
+    amount double,
+    feature float array not null,
+    feature_id bigint not null,
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=64, ncentroids=0, nsubvector=4, nbitsPerIdx=4),
+    primary key(id)
+)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR 9001 (45000): ivf_pq_parameter.ncentroids is illegal : 0 default : 2048</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>create table neg_587 (
     id bigint auto_increment not null, 
     name varchar(32),
@@ -6560,13 +6957,9 @@
     amount double,
     feature float array not null,
     feature_id bigint not null,
-    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=8, ncentroids=64, nsubvector=10, nbits_per_idx=8),
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=8, ncentroids=64, nsubvector=10, nbitsPerIdx=8),
     primary key(id)
 )</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR 9001 (45000): ivf_pq_parameter vector_index_parameter is illegal, dimension:64 / nsubvector:5 not divisible</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6577,81 +6970,9 @@
     amount double,
     feature float array not null,
     feature_id bigint not null,
-    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=64, ncentroids=16, nsubvector=5, nbits_per_idx=8),
+    index feature_index vector(feature_id, feature) parameters(type=ivfpq, metricType=L2, dimension=64, ncentroids=16, nsubvector=5, nbitsPerIdx=8),
     primary key(id)
 )</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(2,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', '0')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(3,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', '1')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(4,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 'true')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(5,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 'False')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(6,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', true1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(7,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', isFalse)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(8,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', isTrue)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(9,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', False0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(10,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07',-2.5)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(11,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07',1.4)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(12,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 0.5)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(13,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 0.0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>布尔字段类型名称为bool，创建表失败</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(1,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10')</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(2,'zhangsan',18,23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07', 1, true)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema1 values(3,'zhangsan','abc',23.50,'beijing','1998-04-06','08:10:10','2022-04-08 18:05:07',true)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema7 values(2,'Li Si','male','1998-03-15',null,5)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $array10 values(407,'zhangsan',18,23.5,array[2.5])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7036,10 +7357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K589"/>
+  <dimension ref="A1:K604"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A389" workbookViewId="0">
-      <selection activeCell="G508" sqref="G508"/>
+    <sheetView tabSelected="1" topLeftCell="D597" workbookViewId="0">
+      <selection activeCell="I598" sqref="I598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12919,7 +13240,7 @@
         <v>1015</v>
       </c>
       <c r="I226" s="1" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
       <c r="J226" s="1" t="s">
         <v>666</v>
@@ -12948,7 +13269,7 @@
         <v>1015</v>
       </c>
       <c r="I227" s="1" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
       <c r="J227" s="1" t="s">
         <v>666</v>
@@ -12977,7 +13298,7 @@
         <v>1015</v>
       </c>
       <c r="I228" s="1" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="J228" s="1" t="s">
         <v>666</v>
@@ -13006,7 +13327,7 @@
         <v>1015</v>
       </c>
       <c r="I229" s="1" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
       <c r="J229" s="1" t="s">
         <v>666</v>
@@ -13035,7 +13356,7 @@
         <v>1015</v>
       </c>
       <c r="I230" s="1" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="J230" s="1" t="s">
         <v>675</v>
@@ -13064,7 +13385,7 @@
         <v>1015</v>
       </c>
       <c r="I231" s="1" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="J231" s="1" t="s">
         <v>676</v>
@@ -13093,7 +13414,7 @@
         <v>1015</v>
       </c>
       <c r="I232" s="1" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="J232" s="1" t="s">
         <v>677</v>
@@ -13122,7 +13443,7 @@
         <v>1015</v>
       </c>
       <c r="I233" s="1" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="J233" s="1" t="s">
         <v>678</v>
@@ -13151,7 +13472,7 @@
         <v>1015</v>
       </c>
       <c r="I234" s="1" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="J234" s="1" t="s">
         <v>679</v>
@@ -13180,7 +13501,7 @@
         <v>1015</v>
       </c>
       <c r="I235" s="1" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="J235" s="1" t="s">
         <v>679</v>
@@ -13209,7 +13530,7 @@
         <v>1015</v>
       </c>
       <c r="I236" s="1" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="J236" s="1" t="s">
         <v>679</v>
@@ -13238,7 +13559,7 @@
         <v>1015</v>
       </c>
       <c r="I237" s="1" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="J237" s="1" t="s">
         <v>679</v>
@@ -13255,7 +13576,7 @@
         <v>25</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>663</v>
@@ -15771,7 +16092,7 @@
         <v>1015</v>
       </c>
       <c r="I311" s="1" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="J311" s="1" t="s">
         <v>928</v>
@@ -15800,7 +16121,7 @@
         <v>1015</v>
       </c>
       <c r="I312" s="1" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="J312" s="1" t="s">
         <v>929</v>
@@ -15829,7 +16150,7 @@
         <v>1015</v>
       </c>
       <c r="I313" s="1" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="J313" s="1" t="s">
         <v>931</v>
@@ -15913,7 +16234,7 @@
         <v>1017</v>
       </c>
       <c r="I316" s="1" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="J316" s="1" t="s">
         <v>958</v>
@@ -18710,7 +19031,7 @@
         <v>1109</v>
       </c>
       <c r="I408" s="1" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="J408" s="1" t="s">
         <v>1261</v>
@@ -23909,7 +24230,7 @@
         <v>1681</v>
       </c>
       <c r="I588" s="5" t="s">
-        <v>1740</v>
+        <v>1818</v>
       </c>
       <c r="J588" s="1" t="s">
         <v>1739</v>
@@ -23935,12 +24256,420 @@
         <v>1681</v>
       </c>
       <c r="I589" s="5" t="s">
-        <v>1742</v>
+        <v>1819</v>
       </c>
       <c r="J589" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="K589" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="590" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A590" s="1" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C590" s="1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D590" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E590" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="F590" s="6" t="s">
+        <v>1767</v>
+      </c>
+      <c r="G590" s="6" t="s">
+        <v>1766</v>
+      </c>
+      <c r="I590" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="J590" s="1" t="s">
+        <v>1769</v>
+      </c>
+      <c r="K590" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="591" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A591" s="1" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B591" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C591" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="D591" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E591" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="F591" s="6" t="s">
+        <v>1767</v>
+      </c>
+      <c r="H591" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="I591" s="1" t="s">
+        <v>1772</v>
+      </c>
+      <c r="J591" s="1" t="s">
+        <v>1773</v>
+      </c>
+      <c r="K591" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="592" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A592" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B592" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C592" s="1" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D592" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E592" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="F592" s="6" t="s">
+        <v>1767</v>
+      </c>
+      <c r="H592" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="I592" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="J592" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="K592" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="593" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A593" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B593" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C593" s="1" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D593" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E593" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="F593" s="6" t="s">
+        <v>1767</v>
+      </c>
+      <c r="H593" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="I593" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="J593" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="K593" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="594" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A594" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B594" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C594" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="D594" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E594" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I594" s="5" t="s">
+        <v>1782</v>
+      </c>
+      <c r="J594" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="K594" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="595" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A595" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B595" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C595" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="D595" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E595" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I595" s="5" t="s">
+        <v>1785</v>
+      </c>
+      <c r="J595" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="K595" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="596" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A596" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B596" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C596" s="1" t="s">
+        <v>1787</v>
+      </c>
+      <c r="D596" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E596" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I596" s="5" t="s">
+        <v>1789</v>
+      </c>
+      <c r="J596" s="1" t="s">
+        <v>1790</v>
+      </c>
+      <c r="K596" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="597" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A597" s="1" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B597" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C597" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="D597" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E597" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I597" s="5" t="s">
+        <v>1791</v>
+      </c>
+      <c r="K597" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="598" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A598" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B598" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C598" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D598" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E598" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I598" s="5" t="s">
+        <v>1795</v>
+      </c>
+      <c r="J598" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="K598" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="599" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A599" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B599" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="D599" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E599" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I599" s="5" t="s">
+        <v>1798</v>
+      </c>
+      <c r="J599" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="K599" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="600" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A600" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B600" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="D600" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E600" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I600" s="5" t="s">
+        <v>1801</v>
+      </c>
+      <c r="K600" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="601" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A601" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B601" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C601" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D601" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E601" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I601" s="5" t="s">
+        <v>1805</v>
+      </c>
+      <c r="J601" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="K601" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="602" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A602" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B602" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="D602" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E602" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I602" s="5" t="s">
+        <v>1809</v>
+      </c>
+      <c r="J602" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="K602" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="603" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A603" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B603" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C603" s="1" t="s">
+        <v>1812</v>
+      </c>
+      <c r="D603" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E603" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I603" s="5" t="s">
+        <v>1811</v>
+      </c>
+      <c r="J603" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="K603" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="604" spans="1:11" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A604" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B604" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D604" s="1" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E604" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="I604" s="5" t="s">
+        <v>1816</v>
+      </c>
+      <c r="J604" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="K604" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
enable case about chinese column definition
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/negative/sql_negative_cases.xlsx
@@ -7359,8 +7359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K604"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D597" workbookViewId="0">
-      <selection activeCell="I598" sqref="I598"/>
+    <sheetView tabSelected="1" topLeftCell="A588" workbookViewId="0">
+      <selection activeCell="G589" sqref="G589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>